<commit_message>
added 0 ohm jumper
</commit_message>
<xml_diff>
--- a/hardware/Hybrid Driver/BOM_hybrid_driver_v1.3_single_pricing.xlsx
+++ b/hardware/Hybrid Driver/BOM_hybrid_driver_v1.3_single_pricing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Quantity</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>Al capacitors should be one of the following brands: Rubycon, Nichicon Panasonic, Mallory, or Sanyo/Nippon</t>
+  </si>
+  <si>
+    <t>0.0QBK-ND</t>
+  </si>
+  <si>
+    <t>0 OHM 1/4W JUMP</t>
+  </si>
+  <si>
+    <t>ZOR-25-B-52-0R</t>
   </si>
 </sst>
 </file>
@@ -293,13 +302,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -321,7 +331,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -332,6 +342,7 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -664,7 +675,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -729,7 +740,7 @@
         <v>0.52</v>
       </c>
       <c r="H2" s="5">
-        <f t="shared" ref="H2:H13" si="0">G2*B2</f>
+        <f t="shared" ref="H2:H14" si="0">G2*B2</f>
         <v>1.04</v>
       </c>
     </row>
@@ -954,26 +965,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G11" s="5">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="0"/>
-        <v>0.27</v>
+        <f t="shared" ref="H11" si="1">G11*B11</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -981,26 +992,26 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G12" s="5">
-        <v>21.74</v>
+        <v>0.27</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="0"/>
-        <v>43.48</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1011,46 +1022,73 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G13" s="5">
-        <v>14.76</v>
+        <v>21.74</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="0"/>
+        <v>43.48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="5">
+        <v>14.76</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="0"/>
         <v>29.52</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="G14" s="8" t="s">
+    <row r="15" spans="1:8">
+      <c r="G15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="9">
-        <f>SUM(H2:H13)</f>
-        <v>79.949999999999989</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="C16" s="1" t="s">
+      <c r="H15" s="9">
+        <f>SUM(H2:H14)</f>
+        <v>80.149999999999991</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1065,9 +1103,10 @@
     <hyperlink ref="C8" r:id="rId7"/>
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C12" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="C11" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>